<commit_message>
Build a 4 bus case for TDSCR
</commit_message>
<xml_diff>
--- a/system_cases/Examples/ParticipationAnalysis/ModalConfig_UserData.xlsx
+++ b/system_cases/Examples/ParticipationAnalysis/ModalConfig_UserData.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Git\Simplex-Power-Systems-2\Examples\ParticipationAnalysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitRep\Simplus-Grid-Tool\system_cases\Examples\ParticipationAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E31E6D0-B0D8-443D-A87F-2B2BE7A89D0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF63E444-6D66-48FE-AAB7-CAE29FE4C9C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{118C985D-F674-4C5E-A300-55E73EA7959C}"/>
+    <workbookView xWindow="4760" yWindow="3730" windowWidth="28800" windowHeight="15370" activeTab="2" xr2:uid="{118C985D-F674-4C5E-A300-55E73EA7959C}"/>
   </bookViews>
   <sheets>
-    <sheet name="State-PF" sheetId="54" r:id="rId1"/>
-    <sheet name="Impedance-PF" sheetId="55" r:id="rId2"/>
-    <sheet name="Enabling" sheetId="56" r:id="rId3"/>
-    <sheet name="SensitivitySel" sheetId="57" r:id="rId4"/>
+    <sheet name="State-PF" sheetId="58" r:id="rId1"/>
+    <sheet name="Impedance-PF" sheetId="59" r:id="rId2"/>
+    <sheet name="Enabling" sheetId="60" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="152">
   <si>
     <t>Select states for state participation analysis. Only 1 mode should be selected.</t>
   </si>
@@ -491,7 +490,7 @@
     <t>Impedance-PF Layer 3</t>
   </si>
   <si>
-    <t>Mode selection for eigenvalue sensitivity analysis</t>
+    <t>whole-system sensitivity</t>
   </si>
 </sst>
 </file>
@@ -842,26 +841,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{171E2CCD-09AE-449C-83DB-7D0D13C5E051}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B608FAC-5738-422A-869A-3BDCE14866EE}">
   <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:G71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -881,7 +880,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -901,7 +900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -918,7 +917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>12</v>
       </c>
@@ -935,7 +934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>14</v>
       </c>
@@ -952,7 +951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>16</v>
       </c>
@@ -969,7 +968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -989,7 +988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -1006,7 +1005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>12</v>
       </c>
@@ -1023,7 +1022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>14</v>
       </c>
@@ -1040,7 +1039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>16</v>
       </c>
@@ -1057,7 +1056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1077,7 +1076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>10</v>
       </c>
@@ -1094,7 +1093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>12</v>
       </c>
@@ -1111,7 +1110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>14</v>
       </c>
@@ -1128,7 +1127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>16</v>
       </c>
@@ -1145,7 +1144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -1165,7 +1164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>10</v>
       </c>
@@ -1182,7 +1181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>12</v>
       </c>
@@ -1199,7 +1198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>48</v>
       </c>
@@ -1216,7 +1215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>51</v>
       </c>
@@ -1233,7 +1232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>54</v>
       </c>
@@ -1250,7 +1249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>14</v>
       </c>
@@ -1267,7 +1266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>16</v>
       </c>
@@ -1284,7 +1283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>60</v>
       </c>
@@ -1301,7 +1300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>63</v>
       </c>
@@ -1318,7 +1317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>66</v>
       </c>
@@ -1338,7 +1337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>70</v>
       </c>
@@ -1355,7 +1354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>73</v>
       </c>
@@ -1372,7 +1371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>76</v>
       </c>
@@ -1389,7 +1388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>79</v>
       </c>
@@ -1406,7 +1405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>81</v>
       </c>
@@ -1420,10 +1419,10 @@
         <v>83</v>
       </c>
       <c r="G37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>73</v>
       </c>
@@ -1440,7 +1439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>76</v>
       </c>
@@ -1454,10 +1453,10 @@
         <v>87</v>
       </c>
       <c r="G39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>79</v>
       </c>
@@ -1474,7 +1473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>81</v>
       </c>
@@ -1491,7 +1490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>73</v>
       </c>
@@ -1508,7 +1507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>76</v>
       </c>
@@ -1525,7 +1524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>73</v>
       </c>
@@ -1542,7 +1541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>76</v>
       </c>
@@ -1559,7 +1558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>97</v>
       </c>
@@ -1576,7 +1575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>100</v>
       </c>
@@ -1593,7 +1592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
         <v>103</v>
       </c>
@@ -1610,7 +1609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>105</v>
       </c>
@@ -1627,7 +1626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
         <v>103</v>
       </c>
@@ -1644,7 +1643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
         <v>105</v>
       </c>
@@ -1661,7 +1660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
         <v>79</v>
       </c>
@@ -1678,7 +1677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
         <v>81</v>
       </c>
@@ -1695,7 +1694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
         <v>103</v>
       </c>
@@ -1712,7 +1711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
         <v>105</v>
       </c>
@@ -1729,7 +1728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
         <v>79</v>
       </c>
@@ -1746,7 +1745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
         <v>81</v>
       </c>
@@ -1763,7 +1762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
         <v>103</v>
       </c>
@@ -1780,7 +1779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
         <v>105</v>
       </c>
@@ -1797,7 +1796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
         <v>117</v>
       </c>
@@ -1814,7 +1813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
         <v>119</v>
       </c>
@@ -1831,7 +1830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
         <v>121</v>
       </c>
@@ -1848,7 +1847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
         <v>123</v>
       </c>
@@ -1865,7 +1864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
         <v>121</v>
       </c>
@@ -1882,7 +1881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B65" t="s">
         <v>123</v>
       </c>
@@ -1899,7 +1898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B66" t="s">
         <v>121</v>
       </c>
@@ -1916,7 +1915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
         <v>123</v>
       </c>
@@ -1933,7 +1932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B68" t="s">
         <v>121</v>
       </c>
@@ -1950,7 +1949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B69" t="s">
         <v>123</v>
       </c>
@@ -1967,7 +1966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B70" t="s">
         <v>131</v>
       </c>
@@ -1984,7 +1983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B71" t="s">
         <v>133</v>
       </c>
@@ -2007,26 +2006,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9040FCB5-ED49-4E04-B21E-3644353E4C4A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49FC817D-F234-4846-A3E3-E887084C969D}">
   <dimension ref="A1:L72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:L72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>136</v>
       </c>
@@ -2040,7 +2039,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -2069,7 +2068,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2080,7 +2079,7 @@
         <v>141</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" t="s">
         <v>9</v>
@@ -2095,10 +2094,10 @@
         <v>7</v>
       </c>
       <c r="L8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -2127,7 +2126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -2156,7 +2155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -2185,7 +2184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="G12" t="s">
         <v>17</v>
       </c>
@@ -2196,7 +2195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="G13" t="s">
         <v>20</v>
       </c>
@@ -2207,7 +2206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="G14" t="s">
         <v>22</v>
       </c>
@@ -2218,7 +2217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="G15" t="s">
         <v>24</v>
       </c>
@@ -2229,7 +2228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="G16" t="s">
         <v>26</v>
       </c>
@@ -2240,7 +2239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G17" t="s">
         <v>28</v>
       </c>
@@ -2251,7 +2250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G18" t="s">
         <v>31</v>
       </c>
@@ -2262,7 +2261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G19" t="s">
         <v>33</v>
       </c>
@@ -2273,7 +2272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G20" t="s">
         <v>35</v>
       </c>
@@ -2284,7 +2283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G21" t="s">
         <v>37</v>
       </c>
@@ -2295,7 +2294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G22" t="s">
         <v>39</v>
       </c>
@@ -2306,7 +2305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G23" t="s">
         <v>42</v>
       </c>
@@ -2317,7 +2316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G24" t="s">
         <v>44</v>
       </c>
@@ -2328,7 +2327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G25" t="s">
         <v>46</v>
       </c>
@@ -2339,7 +2338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G26" t="s">
         <v>49</v>
       </c>
@@ -2350,7 +2349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G27" t="s">
         <v>52</v>
       </c>
@@ -2361,7 +2360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G28" t="s">
         <v>55</v>
       </c>
@@ -2372,7 +2371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G29" t="s">
         <v>56</v>
       </c>
@@ -2383,7 +2382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G30" t="s">
         <v>58</v>
       </c>
@@ -2394,7 +2393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G31" t="s">
         <v>61</v>
       </c>
@@ -2405,7 +2404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G32" t="s">
         <v>64</v>
       </c>
@@ -2416,7 +2415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G33" t="s">
         <v>68</v>
       </c>
@@ -2427,7 +2426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G34" t="s">
         <v>71</v>
       </c>
@@ -2438,7 +2437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G35" t="s">
         <v>74</v>
       </c>
@@ -2449,7 +2448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G36" t="s">
         <v>77</v>
       </c>
@@ -2460,7 +2459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G37" t="s">
         <v>80</v>
       </c>
@@ -2471,7 +2470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G38" t="s">
         <v>82</v>
       </c>
@@ -2479,10 +2478,10 @@
         <v>83</v>
       </c>
       <c r="I38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="7:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G39" t="s">
         <v>84</v>
       </c>
@@ -2493,7 +2492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G40" t="s">
         <v>86</v>
       </c>
@@ -2501,10 +2500,10 @@
         <v>87</v>
       </c>
       <c r="I40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="7:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G41" t="s">
         <v>88</v>
       </c>
@@ -2515,7 +2514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G42" t="s">
         <v>90</v>
       </c>
@@ -2526,7 +2525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G43" t="s">
         <v>92</v>
       </c>
@@ -2537,7 +2536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G44" t="s">
         <v>94</v>
       </c>
@@ -2548,7 +2547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G45" t="s">
         <v>95</v>
       </c>
@@ -2559,7 +2558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G46" t="s">
         <v>96</v>
       </c>
@@ -2570,7 +2569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G47" t="s">
         <v>98</v>
       </c>
@@ -2581,7 +2580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G48" t="s">
         <v>101</v>
       </c>
@@ -2592,7 +2591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G49" t="s">
         <v>104</v>
       </c>
@@ -2603,7 +2602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G50" t="s">
         <v>106</v>
       </c>
@@ -2614,7 +2613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G51" t="s">
         <v>107</v>
       </c>
@@ -2625,7 +2624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G52" t="s">
         <v>108</v>
       </c>
@@ -2636,7 +2635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G53" t="s">
         <v>109</v>
       </c>
@@ -2647,7 +2646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G54" t="s">
         <v>110</v>
       </c>
@@ -2658,7 +2657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G55" t="s">
         <v>111</v>
       </c>
@@ -2669,7 +2668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G56" t="s">
         <v>112</v>
       </c>
@@ -2680,7 +2679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G57" t="s">
         <v>113</v>
       </c>
@@ -2691,7 +2690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G58" t="s">
         <v>114</v>
       </c>
@@ -2702,7 +2701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G59" t="s">
         <v>115</v>
       </c>
@@ -2713,7 +2712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G60" t="s">
         <v>116</v>
       </c>
@@ -2724,7 +2723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G61" t="s">
         <v>118</v>
       </c>
@@ -2735,7 +2734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G62" t="s">
         <v>120</v>
       </c>
@@ -2746,7 +2745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G63" t="s">
         <v>122</v>
       </c>
@@ -2757,7 +2756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G64" t="s">
         <v>124</v>
       </c>
@@ -2768,7 +2767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G65" t="s">
         <v>125</v>
       </c>
@@ -2779,7 +2778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G66" t="s">
         <v>126</v>
       </c>
@@ -2790,7 +2789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G67" t="s">
         <v>127</v>
       </c>
@@ -2801,7 +2800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G68" t="s">
         <v>128</v>
       </c>
@@ -2812,7 +2811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G69" t="s">
         <v>129</v>
       </c>
@@ -2823,7 +2822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G70" t="s">
         <v>130</v>
       </c>
@@ -2834,7 +2833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G71" t="s">
         <v>132</v>
       </c>
@@ -2845,7 +2844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G72" t="s">
         <v>134</v>
       </c>
@@ -2862,26 +2861,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{861AA6A8-740A-46D8-88F0-5E429EF9B112}">
-  <dimension ref="A1:B10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B480D5-D2D9-4F29-B79F-8E971240D1F0}">
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>146</v>
       </c>
@@ -2889,7 +2888,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>147</v>
       </c>
@@ -2897,7 +2896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>148</v>
       </c>
@@ -2905,7 +2904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>149</v>
       </c>
@@ -2913,7 +2912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>150</v>
       </c>
@@ -2921,750 +2920,12 @@
         <v>1</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F59E610-977B-4A84-B06A-9EBA54BC99EC}">
-  <dimension ref="A1:C67"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C67"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23">
-        <v>-300.48</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>56</v>
-      </c>
-      <c r="B24" t="s">
-        <v>57</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>58</v>
-      </c>
-      <c r="B25" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>61</v>
-      </c>
-      <c r="B26" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>64</v>
-      </c>
-      <c r="B27" t="s">
-        <v>65</v>
-      </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>68</v>
-      </c>
-      <c r="B28" t="s">
-        <v>69</v>
-      </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>71</v>
-      </c>
-      <c r="B29" t="s">
-        <v>72</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>74</v>
-      </c>
-      <c r="B30" t="s">
-        <v>75</v>
-      </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>77</v>
-      </c>
-      <c r="B31" t="s">
-        <v>78</v>
-      </c>
-      <c r="C31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>80</v>
-      </c>
-      <c r="B32">
-        <v>-5.2</v>
-      </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>82</v>
-      </c>
-      <c r="B33" t="s">
-        <v>83</v>
-      </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>84</v>
-      </c>
-      <c r="B34" t="s">
-        <v>85</v>
-      </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>86</v>
-      </c>
-      <c r="B35" t="s">
-        <v>87</v>
-      </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>88</v>
-      </c>
-      <c r="B36" t="s">
-        <v>89</v>
-      </c>
-      <c r="C36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>90</v>
-      </c>
-      <c r="B37" t="s">
-        <v>91</v>
-      </c>
-      <c r="C37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>92</v>
-      </c>
-      <c r="B38" t="s">
-        <v>93</v>
-      </c>
-      <c r="C38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>94</v>
-      </c>
-      <c r="B39">
-        <v>-1.59</v>
-      </c>
-      <c r="C39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>95</v>
-      </c>
-      <c r="B40">
-        <v>0</v>
-      </c>
-      <c r="C40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>96</v>
-      </c>
-      <c r="B41">
-        <v>-0.04</v>
-      </c>
-      <c r="C41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>98</v>
-      </c>
-      <c r="B42" t="s">
-        <v>99</v>
-      </c>
-      <c r="C42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>101</v>
-      </c>
-      <c r="B43" t="s">
-        <v>102</v>
-      </c>
-      <c r="C43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>104</v>
-      </c>
-      <c r="B44" t="s">
-        <v>99</v>
-      </c>
-      <c r="C44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>106</v>
-      </c>
-      <c r="B45" t="s">
-        <v>102</v>
-      </c>
-      <c r="C45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>107</v>
-      </c>
-      <c r="B46" t="s">
-        <v>99</v>
-      </c>
-      <c r="C46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>108</v>
-      </c>
-      <c r="B47" t="s">
-        <v>102</v>
-      </c>
-      <c r="C47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>109</v>
-      </c>
-      <c r="B48" t="s">
-        <v>99</v>
-      </c>
-      <c r="C48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>110</v>
-      </c>
-      <c r="B49" t="s">
-        <v>102</v>
-      </c>
-      <c r="C49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>111</v>
-      </c>
-      <c r="B50" t="s">
-        <v>99</v>
-      </c>
-      <c r="C50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>112</v>
-      </c>
-      <c r="B51" t="s">
-        <v>102</v>
-      </c>
-      <c r="C51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>113</v>
-      </c>
-      <c r="B52" t="s">
-        <v>99</v>
-      </c>
-      <c r="C52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>114</v>
-      </c>
-      <c r="B53" t="s">
-        <v>102</v>
-      </c>
-      <c r="C53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>115</v>
-      </c>
-      <c r="B54" t="s">
-        <v>99</v>
-      </c>
-      <c r="C54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>116</v>
-      </c>
-      <c r="B55" t="s">
-        <v>102</v>
-      </c>
-      <c r="C55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>118</v>
-      </c>
-      <c r="B56" t="s">
-        <v>99</v>
-      </c>
-      <c r="C56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>120</v>
-      </c>
-      <c r="B57" t="s">
-        <v>102</v>
-      </c>
-      <c r="C57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>122</v>
-      </c>
-      <c r="B58" t="s">
-        <v>99</v>
-      </c>
-      <c r="C58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>124</v>
-      </c>
-      <c r="B59" t="s">
-        <v>102</v>
-      </c>
-      <c r="C59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>125</v>
-      </c>
-      <c r="B60" t="s">
-        <v>99</v>
-      </c>
-      <c r="C60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>126</v>
-      </c>
-      <c r="B61" t="s">
-        <v>102</v>
-      </c>
-      <c r="C61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>127</v>
-      </c>
-      <c r="B62" t="s">
-        <v>99</v>
-      </c>
-      <c r="C62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>128</v>
-      </c>
-      <c r="B63" t="s">
-        <v>102</v>
-      </c>
-      <c r="C63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>129</v>
-      </c>
-      <c r="B64" t="s">
-        <v>99</v>
-      </c>
-      <c r="C64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>130</v>
-      </c>
-      <c r="B65" t="s">
-        <v>102</v>
-      </c>
-      <c r="C65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>132</v>
-      </c>
-      <c r="B66" t="s">
-        <v>99</v>
-      </c>
-      <c r="C66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>134</v>
-      </c>
-      <c r="B67" t="s">
-        <v>102</v>
-      </c>
-      <c r="C67">
-        <v>0</v>
+      <c r="B11">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>